<commit_message>
Tạo role Staff, Manager
</commit_message>
<xml_diff>
--- a/Database/ACL.xlsx
+++ b/Database/ACL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\22110006_VI_QUỐC_THUẬN\HKI_NĂM_3\HỆ QUẢN TRỊ CSDL\DOANCUOIKY\FashionShopManagement\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B90F2F5-06B5-494A-874A-65CCEA16F319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3134C77C-B412-4C92-8454-EAAAAA5045DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F1F942E8-D06A-40FE-A0D6-E2765517E40E}"/>
   </bookViews>
@@ -251,7 +251,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE67D137-E849-4D65-873C-2E4CF7955C08}" name="Table1" displayName="Table1" ref="F4:K48" totalsRowShown="0">
-  <autoFilter ref="F4:K48" xr:uid="{BE67D137-E849-4D65-873C-2E4CF7955C08}"/>
+  <autoFilter ref="F4:K48" xr:uid="{BE67D137-E849-4D65-873C-2E4CF7955C08}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="x"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EDDA0BB4-E488-4416-86D9-90C72726D3C1}" name="ROLE"/>
     <tableColumn id="2" xr3:uid="{3EDEB4F8-5B22-44B7-BF02-C097B15FD855}" name="SP"/>
@@ -583,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBDBB32-F66C-40B6-98D3-ECB51EA40B7A}">
   <dimension ref="F4:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,7 +621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -623,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
         <v>2</v>
       </c>
@@ -631,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F7" t="s">
         <v>2</v>
       </c>
@@ -639,7 +645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>2</v>
       </c>
@@ -647,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>2</v>
       </c>
@@ -655,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F10" t="s">
         <v>2</v>
       </c>
@@ -663,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
         <v>2</v>
       </c>
@@ -671,7 +677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
         <v>2</v>
       </c>
@@ -712,7 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>2</v>
       </c>
@@ -720,7 +726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F17" t="s">
         <v>2</v>
       </c>
@@ -739,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F19" t="s">
         <v>2</v>
       </c>
@@ -783,7 +789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
         <v>2</v>
       </c>
@@ -915,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F35" t="s">
         <v>2</v>
       </c>
@@ -945,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F38" t="s">
         <v>2</v>
       </c>
@@ -953,7 +959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F39" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="6:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="F48" t="s">
         <v>2</v>
       </c>

</xml_diff>